<commit_message>
Performer Process is complete
</commit_message>
<xml_diff>
--- a/GenerateYearlyReport_Performer/Data/Config.xlsx
+++ b/GenerateYearlyReport_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bioni\Development\UIPathAcademy\UiPathAcademy\GenerateYearlyReport_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098701D7-2A98-4097-9174-47E79B8592A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BEDAEF-E32C-43FB-A73C-51E7FA9E9BFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1110" windowWidth="24930" windowHeight="13935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="1110" windowWidth="24930" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -177,13 +177,13 @@
     <t>ACMELogin</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/account/login</t>
-  </si>
-  <si>
     <t>ReportsDownloadPath</t>
   </si>
   <si>
     <t>Data\Temp</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
   </si>
 </sst>
 </file>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -637,10 +637,10 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1644,7 +1644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>